<commit_message>
changed biosampleNumber to bioSampleNumber in rnaSample
</commit_message>
<xml_diff>
--- a/bioSample/bioSample_hbrown_01.29.20.xlsx
+++ b/bioSample/bioSample_hbrown_01.29.20.xlsx
@@ -22,7 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="25">
   <si>
-    <t xml:space="preserve">inductionDate</t>
+    <t xml:space="preserve">harvestDate</t>
   </si>
   <si>
     <t xml:space="preserve">harvester</t>
@@ -104,7 +104,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -126,12 +126,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -188,11 +182,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -216,16 +210,18 @@
   <dimension ref="A1:Z27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="10.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="5" style="0" width="10.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="17.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="10.61"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>